<commit_message>
some other improvements and fixes there is now some basic support for data types
</commit_message>
<xml_diff>
--- a/templates/spec.xlsx
+++ b/templates/spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>a</t>
   </si>
@@ -30,11 +30,25 @@
   <si>
     <t>c</t>
   </si>
+  <si>
+    <t>formats</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>last row is 11, 8 rows are in use (row_count)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -64,8 +78,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,30 +434,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="G3" s="6">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -446,6 +478,29 @@
       </c>
       <c r="C4" t="s">
         <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="G5" s="1">
+        <v>40762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="G6" s="2">
+        <v>40762.022222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" s="3">
+        <v>40762.063888888901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>